<commit_message>
catch up un mes
</commit_message>
<xml_diff>
--- a/experimento1.xlsx
+++ b/experimento1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgarciay/Desktop/Laval_Master_Computer/research/Synthetic-Data-Deep-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7326F8D4-AE71-0847-821D-6F4E93D00DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E79123F-3E8F-B64A-826A-F68514563838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="2920" windowWidth="27580" windowHeight="16660" activeTab="2" xr2:uid="{DFB239C8-EEA5-3943-A44C-3A2C10E6A7DD}"/>
+    <workbookView xWindow="10820" yWindow="2920" windowWidth="27580" windowHeight="16660" activeTab="2" xr2:uid="{DFB239C8-EEA5-3943-A44C-3A2C10E6A7DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Visit" sheetId="4" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="136">
   <si>
     <t>Num Cluster</t>
   </si>
@@ -713,9 +713,6 @@
     <t>running</t>
   </si>
   <si>
-    <t>falta verificar resultados. Y descargarlos</t>
-  </si>
-  <si>
     <t>done/faltan verificar imagens</t>
   </si>
   <si>
@@ -729,7 +726,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -839,12 +836,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1264,14 +1255,14 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3050,25 +3041,25 @@
     <cfRule type="top10" dxfId="19" priority="28" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D1048576 D1">
-    <cfRule type="top10" dxfId="18" priority="26" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="17" priority="29" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="18" priority="29" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="17" priority="26" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:P1">
-    <cfRule type="top10" dxfId="16" priority="20" rank="3"/>
-    <cfRule type="top10" dxfId="15" priority="21" rank="2"/>
-    <cfRule type="top10" dxfId="14" priority="22" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="21" rank="2"/>
+    <cfRule type="top10" dxfId="15" priority="22" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="20" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:P8">
-    <cfRule type="top10" dxfId="13" priority="23" rank="3"/>
-    <cfRule type="top10" dxfId="12" priority="24" rank="2"/>
+    <cfRule type="top10" dxfId="13" priority="24" rank="2"/>
+    <cfRule type="top10" dxfId="12" priority="23" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:P1048576">
     <cfRule type="top10" dxfId="11" priority="25" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AU2">
-    <cfRule type="top10" dxfId="10" priority="14" rank="3"/>
+    <cfRule type="top10" dxfId="10" priority="16" rank="1"/>
     <cfRule type="top10" dxfId="9" priority="15" rank="2"/>
-    <cfRule type="top10" dxfId="8" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="14" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4939,7 +4930,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4953,9 +4944,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="112"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -4988,10 +4979,10 @@
         <v>112</v>
       </c>
       <c r="B4" s="100" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" s="100"/>
       <c r="E4" s="100" t="s">
@@ -5012,13 +5003,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="100" t="s">
         <v>132</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D5" s="100"/>
       <c r="E5" s="100"/>
@@ -5050,12 +5041,8 @@
       <c r="A7" s="107" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="100" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" s="100" t="s">
-        <v>134</v>
-      </c>
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
       <c r="D7" s="100"/>
       <c r="E7" s="100"/>
       <c r="F7" s="100"/>
@@ -5084,7 +5071,7 @@
       <c r="A9" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="113"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="100" t="s">
         <v>126</v>
       </c>
@@ -5102,10 +5089,10 @@
         <v>112</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10" s="109" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D10" s="109"/>
       <c r="E10" s="109"/>
@@ -5118,14 +5105,12 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="109" t="s">
-        <v>132</v>
-      </c>
+      <c r="C11" s="109"/>
       <c r="D11" s="109"/>
       <c r="E11" s="109"/>
       <c r="F11" s="109"/>
@@ -5155,11 +5140,9 @@
         <v>114</v>
       </c>
       <c r="B13" s="100" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="100" t="s">
-        <v>134</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C13" s="100"/>
       <c r="D13" s="109"/>
       <c r="E13" s="109"/>
       <c r="F13" s="109"/>
@@ -5188,7 +5171,7 @@
       <c r="A15" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="115"/>
+      <c r="B15" s="114"/>
       <c r="C15" s="109" t="s">
         <v>126</v>
       </c>
@@ -5205,37 +5188,35 @@
       <c r="A16" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="114" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" s="114" t="s">
-        <v>135</v>
-      </c>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
-      <c r="H16" s="114"/>
-      <c r="I16" s="114" t="s">
+      <c r="B16" s="113" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="113" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="113" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="101" t="s">
-        <v>136</v>
-      </c>
-      <c r="B17" s="114" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="113" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="114" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="114"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="114"/>
-      <c r="G17" s="114"/>
-      <c r="H17" s="114"/>
-      <c r="I17" s="114" t="s">
+      <c r="C17" s="113"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="113" t="s">
         <v>131</v>
       </c>
     </row>
@@ -5261,9 +5242,7 @@
       <c r="B19" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="110" t="s">
-        <v>132</v>
-      </c>
+      <c r="C19" s="110"/>
       <c r="D19" s="110"/>
       <c r="E19" s="110"/>
       <c r="F19" s="110"/>
@@ -5296,7 +5275,7 @@
       <c r="A21" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="113" t="s">
+      <c r="B21" s="112" t="s">
         <v>133</v>
       </c>
       <c r="C21" s="109" t="s">

</xml_diff>